<commit_message>
UNIT Add button & SBU Data test
</commit_message>
<xml_diff>
--- a/src/test/java/Data/Data.xlsx
+++ b/src/test/java/Data/Data.xlsx
@@ -1,21 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25928"/>
-  <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AUTOMATION-QDMS\QDMS_Automation\src\test\java\Data\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B57C12C-64BD-455B-BB91-2101443306E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="4140" yWindow="1680" windowWidth="15375" windowHeight="7785" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14025" windowHeight="1230" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
+    <sheet name="AddSbu" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:N2"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,21 +21,39 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>admin</t>
   </si>
   <si>
-    <t xml:space="preserve">tokyo@admin </t>
-  </si>
-  <si>
     <t>http://192.168.1.35:8083/#/</t>
+  </si>
+  <si>
+    <t>tokyo@admin</t>
+  </si>
+  <si>
+    <t>CEMENT</t>
+  </si>
+  <si>
+    <t>qqqqq</t>
+  </si>
+  <si>
+    <t>RMC</t>
+  </si>
+  <si>
+    <t>qqqqqqqq</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>qqqqqqqqq</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -361,11 +375,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -378,17 +392,65 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B1" r:id="rId1" xr:uid="{143A726D-C281-474B-95F5-C95061D8399C}"/>
-    <hyperlink ref="C1" r:id="rId2" location="/" xr:uid="{78CB7F41-54EF-459A-80DB-4079ED04B583}"/>
+    <hyperlink ref="B1" r:id="rId1"/>
+    <hyperlink ref="C1" r:id="rId2" location="/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="b">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>